<commit_message>
Change to ESP32 with FastDAC, Wifi
Wifi time synch
#option to switch to Teensy
</commit_message>
<xml_diff>
--- a/Plots.xlsx
+++ b/Plots.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Source Code\Arduino Source Code\O-Scope_XY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC8A048-DE37-43CE-AC85-DB6582BD287B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF05D64-CB8A-4F35-BED2-728D46284E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4021E60-8DFB-4E05-9B04-73E3B9062F1F}"/>
+    <workbookView minimized="1" xWindow="5844" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{A4021E60-8DFB-4E05-9B04-73E3B9062F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cat points" sheetId="7" r:id="rId1"/>
     <sheet name="Tek" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="Trav" sheetId="2" r:id="rId4"/>
-    <sheet name="Tree" sheetId="1" r:id="rId5"/>
-    <sheet name="Clover" sheetId="3" r:id="rId6"/>
-    <sheet name="4  leaf" sheetId="4" r:id="rId7"/>
+    <sheet name="Trav" sheetId="2" r:id="rId3"/>
+    <sheet name="Tree" sheetId="1" r:id="rId4"/>
+    <sheet name="Clover" sheetId="3" r:id="rId5"/>
+    <sheet name="4  leaf" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>x</t>
   </si>
@@ -88,33 +87,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>const</t>
-  </si>
-  <si>
-    <t>unsigned</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>x_points[NUM_POINTS]</t>
-  </si>
-  <si>
-    <t>PROGMEM=</t>
-  </si>
-  <si>
-    <t>115}</t>
-  </si>
-  <si>
-    <t>y_points[NUM_POINTS]</t>
-  </si>
-  <si>
-    <t>PROGMEM</t>
-  </si>
-  <si>
-    <t>70}</t>
   </si>
 </sst>
 </file>
@@ -10040,4872 +10012,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1640025-262B-488B-9CC5-F2E7267BC730}">
-  <dimension ref="C6:MM353"/>
-  <sheetViews>
-    <sheetView topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:E353"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="6" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6">
-        <v>155</v>
-      </c>
-      <c r="I6">
-        <v>153</v>
-      </c>
-      <c r="J6">
-        <v>153</v>
-      </c>
-      <c r="K6">
-        <v>152</v>
-      </c>
-      <c r="L6">
-        <v>151</v>
-      </c>
-      <c r="M6">
-        <v>149</v>
-      </c>
-      <c r="N6">
-        <v>148</v>
-      </c>
-      <c r="O6">
-        <v>146</v>
-      </c>
-      <c r="P6">
-        <v>144</v>
-      </c>
-      <c r="Q6">
-        <v>143</v>
-      </c>
-      <c r="R6">
-        <v>141</v>
-      </c>
-      <c r="S6">
-        <v>139</v>
-      </c>
-      <c r="T6">
-        <v>138</v>
-      </c>
-      <c r="U6">
-        <v>136</v>
-      </c>
-      <c r="V6">
-        <v>134</v>
-      </c>
-      <c r="W6">
-        <v>132</v>
-      </c>
-      <c r="X6">
-        <v>130</v>
-      </c>
-      <c r="Y6">
-        <v>128</v>
-      </c>
-      <c r="Z6">
-        <v>126</v>
-      </c>
-      <c r="AA6">
-        <v>124</v>
-      </c>
-      <c r="AB6">
-        <v>122</v>
-      </c>
-      <c r="AC6">
-        <v>120</v>
-      </c>
-      <c r="AD6">
-        <v>119</v>
-      </c>
-      <c r="AE6">
-        <v>118</v>
-      </c>
-      <c r="AF6">
-        <v>118</v>
-      </c>
-      <c r="AG6">
-        <v>116</v>
-      </c>
-      <c r="AH6">
-        <v>116</v>
-      </c>
-      <c r="AI6">
-        <v>116</v>
-      </c>
-      <c r="AJ6">
-        <v>115</v>
-      </c>
-      <c r="AK6">
-        <v>114</v>
-      </c>
-      <c r="AL6">
-        <v>113</v>
-      </c>
-      <c r="AM6">
-        <v>113</v>
-      </c>
-      <c r="AN6">
-        <v>112</v>
-      </c>
-      <c r="AO6">
-        <v>111</v>
-      </c>
-      <c r="AP6">
-        <v>110</v>
-      </c>
-      <c r="AQ6">
-        <v>109</v>
-      </c>
-      <c r="AR6">
-        <v>107</v>
-      </c>
-      <c r="AS6">
-        <v>106</v>
-      </c>
-      <c r="AT6">
-        <v>105</v>
-      </c>
-      <c r="AU6">
-        <v>104</v>
-      </c>
-      <c r="AV6">
-        <v>103</v>
-      </c>
-      <c r="AW6">
-        <v>103</v>
-      </c>
-      <c r="AX6">
-        <v>102</v>
-      </c>
-      <c r="AY6">
-        <v>101</v>
-      </c>
-      <c r="AZ6">
-        <v>100</v>
-      </c>
-      <c r="BA6">
-        <v>99</v>
-      </c>
-      <c r="BB6">
-        <v>98</v>
-      </c>
-      <c r="BC6">
-        <v>98</v>
-      </c>
-      <c r="BD6">
-        <v>98</v>
-      </c>
-      <c r="BE6">
-        <v>98</v>
-      </c>
-      <c r="BF6">
-        <v>98</v>
-      </c>
-      <c r="BG6">
-        <v>98</v>
-      </c>
-      <c r="BH6">
-        <v>98</v>
-      </c>
-      <c r="BI6">
-        <v>98</v>
-      </c>
-      <c r="BJ6">
-        <v>98</v>
-      </c>
-      <c r="BK6">
-        <v>98</v>
-      </c>
-      <c r="BL6">
-        <v>97</v>
-      </c>
-      <c r="BM6">
-        <v>97</v>
-      </c>
-      <c r="BN6">
-        <v>155</v>
-      </c>
-      <c r="BO6">
-        <v>156</v>
-      </c>
-      <c r="BP6">
-        <v>157</v>
-      </c>
-      <c r="BQ6">
-        <v>157</v>
-      </c>
-      <c r="BR6">
-        <v>158</v>
-      </c>
-      <c r="BS6">
-        <v>159</v>
-      </c>
-      <c r="BT6">
-        <v>160</v>
-      </c>
-      <c r="BU6">
-        <v>161</v>
-      </c>
-      <c r="BV6">
-        <v>162</v>
-      </c>
-      <c r="BW6">
-        <v>162</v>
-      </c>
-      <c r="BX6">
-        <v>164</v>
-      </c>
-      <c r="BY6">
-        <v>165</v>
-      </c>
-      <c r="BZ6">
-        <v>166</v>
-      </c>
-      <c r="CA6">
-        <v>167</v>
-      </c>
-      <c r="CB6">
-        <v>168</v>
-      </c>
-      <c r="CC6">
-        <v>170</v>
-      </c>
-      <c r="CD6">
-        <v>170</v>
-      </c>
-      <c r="CE6">
-        <v>171</v>
-      </c>
-      <c r="CF6">
-        <v>171</v>
-      </c>
-      <c r="CG6">
-        <v>172</v>
-      </c>
-      <c r="CH6">
-        <v>172</v>
-      </c>
-      <c r="CI6">
-        <v>172</v>
-      </c>
-      <c r="CJ6">
-        <v>173</v>
-      </c>
-      <c r="CK6">
-        <v>173</v>
-      </c>
-      <c r="CL6">
-        <v>173</v>
-      </c>
-      <c r="CM6">
-        <v>173</v>
-      </c>
-      <c r="CN6">
-        <v>174</v>
-      </c>
-      <c r="CO6">
-        <v>174</v>
-      </c>
-      <c r="CP6">
-        <v>176</v>
-      </c>
-      <c r="CQ6">
-        <v>176</v>
-      </c>
-      <c r="CR6">
-        <v>176</v>
-      </c>
-      <c r="CS6">
-        <v>177</v>
-      </c>
-      <c r="CT6">
-        <v>177</v>
-      </c>
-      <c r="CU6">
-        <v>177</v>
-      </c>
-      <c r="CV6">
-        <v>177</v>
-      </c>
-      <c r="CW6">
-        <v>177</v>
-      </c>
-      <c r="CX6">
-        <v>177</v>
-      </c>
-      <c r="CY6">
-        <v>177</v>
-      </c>
-      <c r="CZ6">
-        <v>175</v>
-      </c>
-      <c r="DA6">
-        <v>175</v>
-      </c>
-      <c r="DB6">
-        <v>174</v>
-      </c>
-      <c r="DC6">
-        <v>173</v>
-      </c>
-      <c r="DD6">
-        <v>172</v>
-      </c>
-      <c r="DE6">
-        <v>170</v>
-      </c>
-      <c r="DF6">
-        <v>169</v>
-      </c>
-      <c r="DG6">
-        <v>168</v>
-      </c>
-      <c r="DH6">
-        <v>166</v>
-      </c>
-      <c r="DI6">
-        <v>165</v>
-      </c>
-      <c r="DJ6">
-        <v>163</v>
-      </c>
-      <c r="DK6">
-        <v>162</v>
-      </c>
-      <c r="DL6">
-        <v>161</v>
-      </c>
-      <c r="DM6">
-        <v>159</v>
-      </c>
-      <c r="DN6">
-        <v>157</v>
-      </c>
-      <c r="DO6">
-        <v>156</v>
-      </c>
-      <c r="DP6">
-        <v>154</v>
-      </c>
-      <c r="DQ6">
-        <v>152</v>
-      </c>
-      <c r="DR6">
-        <v>150</v>
-      </c>
-      <c r="DS6">
-        <v>149</v>
-      </c>
-      <c r="DT6">
-        <v>147</v>
-      </c>
-      <c r="DU6">
-        <v>145</v>
-      </c>
-      <c r="DV6">
-        <v>143</v>
-      </c>
-      <c r="DW6">
-        <v>141</v>
-      </c>
-      <c r="DX6">
-        <v>139</v>
-      </c>
-      <c r="DY6">
-        <v>137</v>
-      </c>
-      <c r="DZ6">
-        <v>135</v>
-      </c>
-      <c r="EA6">
-        <v>133</v>
-      </c>
-      <c r="EB6">
-        <v>131</v>
-      </c>
-      <c r="EC6">
-        <v>129</v>
-      </c>
-      <c r="ED6">
-        <v>127</v>
-      </c>
-      <c r="EE6">
-        <v>125</v>
-      </c>
-      <c r="EF6">
-        <v>123</v>
-      </c>
-      <c r="EG6">
-        <v>121</v>
-      </c>
-      <c r="EH6">
-        <v>119</v>
-      </c>
-      <c r="EI6">
-        <v>117</v>
-      </c>
-      <c r="EJ6">
-        <v>116</v>
-      </c>
-      <c r="EK6">
-        <v>114</v>
-      </c>
-      <c r="EL6">
-        <v>113</v>
-      </c>
-      <c r="EM6">
-        <v>111</v>
-      </c>
-      <c r="EN6">
-        <v>110</v>
-      </c>
-      <c r="EO6">
-        <v>108</v>
-      </c>
-      <c r="EP6">
-        <v>107</v>
-      </c>
-      <c r="EQ6">
-        <v>106</v>
-      </c>
-      <c r="ER6">
-        <v>105</v>
-      </c>
-      <c r="ES6">
-        <v>104</v>
-      </c>
-      <c r="ET6">
-        <v>103</v>
-      </c>
-      <c r="EU6">
-        <v>102</v>
-      </c>
-      <c r="EV6">
-        <v>101</v>
-      </c>
-      <c r="EW6">
-        <v>100</v>
-      </c>
-      <c r="EX6">
-        <v>99</v>
-      </c>
-      <c r="EY6">
-        <v>98</v>
-      </c>
-      <c r="EZ6">
-        <v>98</v>
-      </c>
-      <c r="FA6">
-        <v>97</v>
-      </c>
-      <c r="FB6">
-        <v>96</v>
-      </c>
-      <c r="FC6">
-        <v>96</v>
-      </c>
-      <c r="FD6">
-        <v>96</v>
-      </c>
-      <c r="FE6">
-        <v>95</v>
-      </c>
-      <c r="FF6">
-        <v>95</v>
-      </c>
-      <c r="FG6">
-        <v>95</v>
-      </c>
-      <c r="FH6">
-        <v>96</v>
-      </c>
-      <c r="FI6">
-        <v>139</v>
-      </c>
-      <c r="FJ6">
-        <v>138</v>
-      </c>
-      <c r="FK6">
-        <v>136</v>
-      </c>
-      <c r="FL6">
-        <v>134</v>
-      </c>
-      <c r="FM6">
-        <v>132</v>
-      </c>
-      <c r="FN6">
-        <v>130</v>
-      </c>
-      <c r="FO6">
-        <v>128</v>
-      </c>
-      <c r="FP6">
-        <v>128</v>
-      </c>
-      <c r="FQ6">
-        <v>129</v>
-      </c>
-      <c r="FR6">
-        <v>130</v>
-      </c>
-      <c r="FS6">
-        <v>131</v>
-      </c>
-      <c r="FT6">
-        <v>132</v>
-      </c>
-      <c r="FU6">
-        <v>134</v>
-      </c>
-      <c r="FV6">
-        <v>135</v>
-      </c>
-      <c r="FW6">
-        <v>137</v>
-      </c>
-      <c r="FX6">
-        <v>139</v>
-      </c>
-      <c r="FY6">
-        <v>140</v>
-      </c>
-      <c r="FZ6">
-        <v>142</v>
-      </c>
-      <c r="GA6">
-        <v>142</v>
-      </c>
-      <c r="GB6">
-        <v>143</v>
-      </c>
-      <c r="GC6">
-        <v>143</v>
-      </c>
-      <c r="GD6">
-        <v>143</v>
-      </c>
-      <c r="GE6">
-        <v>141</v>
-      </c>
-      <c r="GF6">
-        <v>139</v>
-      </c>
-      <c r="GG6">
-        <v>138</v>
-      </c>
-      <c r="GH6">
-        <v>136</v>
-      </c>
-      <c r="GI6">
-        <v>135</v>
-      </c>
-      <c r="GJ6">
-        <v>138</v>
-      </c>
-      <c r="GK6">
-        <v>138</v>
-      </c>
-      <c r="GL6">
-        <v>138</v>
-      </c>
-      <c r="GM6">
-        <v>138</v>
-      </c>
-      <c r="GN6">
-        <v>138</v>
-      </c>
-      <c r="GO6">
-        <v>137</v>
-      </c>
-      <c r="GP6">
-        <v>136</v>
-      </c>
-      <c r="GQ6">
-        <v>134</v>
-      </c>
-      <c r="GR6">
-        <v>132</v>
-      </c>
-      <c r="GS6">
-        <v>130</v>
-      </c>
-      <c r="GT6">
-        <v>129</v>
-      </c>
-      <c r="GU6">
-        <v>139</v>
-      </c>
-      <c r="GV6">
-        <v>139</v>
-      </c>
-      <c r="GW6">
-        <v>139</v>
-      </c>
-      <c r="GX6">
-        <v>139</v>
-      </c>
-      <c r="GY6">
-        <v>139</v>
-      </c>
-      <c r="GZ6">
-        <v>140</v>
-      </c>
-      <c r="HA6">
-        <v>141</v>
-      </c>
-      <c r="HB6">
-        <v>143</v>
-      </c>
-      <c r="HC6">
-        <v>145</v>
-      </c>
-      <c r="HD6">
-        <v>147</v>
-      </c>
-      <c r="HE6">
-        <v>163</v>
-      </c>
-      <c r="HF6">
-        <v>165</v>
-      </c>
-      <c r="HG6">
-        <v>166</v>
-      </c>
-      <c r="HH6">
-        <v>168</v>
-      </c>
-      <c r="HI6">
-        <v>170</v>
-      </c>
-      <c r="HJ6">
-        <v>172</v>
-      </c>
-      <c r="HK6">
-        <v>173</v>
-      </c>
-      <c r="HL6">
-        <v>175</v>
-      </c>
-      <c r="HM6">
-        <v>177</v>
-      </c>
-      <c r="HN6">
-        <v>178</v>
-      </c>
-      <c r="HO6">
-        <v>180</v>
-      </c>
-      <c r="HP6">
-        <v>181</v>
-      </c>
-      <c r="HQ6">
-        <v>183</v>
-      </c>
-      <c r="HR6">
-        <v>185</v>
-      </c>
-      <c r="HS6">
-        <v>186</v>
-      </c>
-      <c r="HT6">
-        <v>188</v>
-      </c>
-      <c r="HU6">
-        <v>190</v>
-      </c>
-      <c r="HV6">
-        <v>191</v>
-      </c>
-      <c r="HW6">
-        <v>193</v>
-      </c>
-      <c r="HX6">
-        <v>195</v>
-      </c>
-      <c r="HY6">
-        <v>197</v>
-      </c>
-      <c r="HZ6">
-        <v>199</v>
-      </c>
-      <c r="IA6">
-        <v>201</v>
-      </c>
-      <c r="IB6">
-        <v>203</v>
-      </c>
-      <c r="IC6">
-        <v>205</v>
-      </c>
-      <c r="ID6">
-        <v>207</v>
-      </c>
-      <c r="IE6">
-        <v>209</v>
-      </c>
-      <c r="IF6">
-        <v>211</v>
-      </c>
-      <c r="IG6">
-        <v>156</v>
-      </c>
-      <c r="IH6">
-        <v>157</v>
-      </c>
-      <c r="II6">
-        <v>158</v>
-      </c>
-      <c r="IJ6">
-        <v>160</v>
-      </c>
-      <c r="IK6">
-        <v>161</v>
-      </c>
-      <c r="IL6">
-        <v>162</v>
-      </c>
-      <c r="IM6">
-        <v>164</v>
-      </c>
-      <c r="IN6">
-        <v>165</v>
-      </c>
-      <c r="IO6">
-        <v>167</v>
-      </c>
-      <c r="IP6">
-        <v>169</v>
-      </c>
-      <c r="IQ6">
-        <v>170</v>
-      </c>
-      <c r="IR6">
-        <v>172</v>
-      </c>
-      <c r="IS6">
-        <v>173</v>
-      </c>
-      <c r="IT6">
-        <v>175</v>
-      </c>
-      <c r="IU6">
-        <v>176</v>
-      </c>
-      <c r="IV6">
-        <v>177</v>
-      </c>
-      <c r="IW6">
-        <v>179</v>
-      </c>
-      <c r="IX6">
-        <v>180</v>
-      </c>
-      <c r="IY6">
-        <v>181</v>
-      </c>
-      <c r="IZ6">
-        <v>183</v>
-      </c>
-      <c r="JA6">
-        <v>184</v>
-      </c>
-      <c r="JB6">
-        <v>186</v>
-      </c>
-      <c r="JC6">
-        <v>187</v>
-      </c>
-      <c r="JD6">
-        <v>188</v>
-      </c>
-      <c r="JE6">
-        <v>189</v>
-      </c>
-      <c r="JF6">
-        <v>190</v>
-      </c>
-      <c r="JG6">
-        <v>191</v>
-      </c>
-      <c r="JH6">
-        <v>152</v>
-      </c>
-      <c r="JI6">
-        <v>153</v>
-      </c>
-      <c r="JJ6">
-        <v>155</v>
-      </c>
-      <c r="JK6">
-        <v>156</v>
-      </c>
-      <c r="JL6">
-        <v>157</v>
-      </c>
-      <c r="JM6">
-        <v>159</v>
-      </c>
-      <c r="JN6">
-        <v>161</v>
-      </c>
-      <c r="JO6">
-        <v>162</v>
-      </c>
-      <c r="JP6">
-        <v>163</v>
-      </c>
-      <c r="JQ6">
-        <v>164</v>
-      </c>
-      <c r="JR6">
-        <v>165</v>
-      </c>
-      <c r="JS6">
-        <v>167</v>
-      </c>
-      <c r="JT6">
-        <v>168</v>
-      </c>
-      <c r="JU6">
-        <v>169</v>
-      </c>
-      <c r="JV6">
-        <v>171</v>
-      </c>
-      <c r="JW6">
-        <v>172</v>
-      </c>
-      <c r="JX6">
-        <v>173</v>
-      </c>
-      <c r="JY6">
-        <v>174</v>
-      </c>
-      <c r="JZ6">
-        <v>175</v>
-      </c>
-      <c r="KA6">
-        <v>114</v>
-      </c>
-      <c r="KB6">
-        <v>112</v>
-      </c>
-      <c r="KC6">
-        <v>110</v>
-      </c>
-      <c r="KD6">
-        <v>109</v>
-      </c>
-      <c r="KE6">
-        <v>107</v>
-      </c>
-      <c r="KF6">
-        <v>106</v>
-      </c>
-      <c r="KG6">
-        <v>105</v>
-      </c>
-      <c r="KH6">
-        <v>103</v>
-      </c>
-      <c r="KI6">
-        <v>102</v>
-      </c>
-      <c r="KJ6">
-        <v>100</v>
-      </c>
-      <c r="KK6">
-        <v>98</v>
-      </c>
-      <c r="KL6">
-        <v>97</v>
-      </c>
-      <c r="KM6">
-        <v>95</v>
-      </c>
-      <c r="KN6">
-        <v>94</v>
-      </c>
-      <c r="KO6">
-        <v>92</v>
-      </c>
-      <c r="KP6">
-        <v>91</v>
-      </c>
-      <c r="KQ6">
-        <v>89</v>
-      </c>
-      <c r="KR6">
-        <v>88</v>
-      </c>
-      <c r="KS6">
-        <v>86</v>
-      </c>
-      <c r="KT6">
-        <v>84</v>
-      </c>
-      <c r="KU6">
-        <v>83</v>
-      </c>
-      <c r="KV6">
-        <v>81</v>
-      </c>
-      <c r="KW6">
-        <v>79</v>
-      </c>
-      <c r="KX6">
-        <v>81</v>
-      </c>
-      <c r="KY6">
-        <v>82</v>
-      </c>
-      <c r="KZ6">
-        <v>84</v>
-      </c>
-      <c r="LA6">
-        <v>86</v>
-      </c>
-      <c r="LB6">
-        <v>88</v>
-      </c>
-      <c r="LC6">
-        <v>120</v>
-      </c>
-      <c r="LD6">
-        <v>118</v>
-      </c>
-      <c r="LE6">
-        <v>117</v>
-      </c>
-      <c r="LF6">
-        <v>116</v>
-      </c>
-      <c r="LG6">
-        <v>115</v>
-      </c>
-      <c r="LH6">
-        <v>114</v>
-      </c>
-      <c r="LI6">
-        <v>114</v>
-      </c>
-      <c r="LJ6">
-        <v>113</v>
-      </c>
-      <c r="LK6">
-        <v>112</v>
-      </c>
-      <c r="LL6">
-        <v>111</v>
-      </c>
-      <c r="LM6">
-        <v>110</v>
-      </c>
-      <c r="LN6">
-        <v>109</v>
-      </c>
-      <c r="LO6">
-        <v>108</v>
-      </c>
-      <c r="LP6">
-        <v>107</v>
-      </c>
-      <c r="LQ6">
-        <v>106</v>
-      </c>
-      <c r="LR6">
-        <v>104</v>
-      </c>
-      <c r="LS6">
-        <v>104</v>
-      </c>
-      <c r="LT6">
-        <v>102</v>
-      </c>
-      <c r="LU6">
-        <v>101</v>
-      </c>
-      <c r="LV6">
-        <v>100</v>
-      </c>
-      <c r="LW6">
-        <v>98</v>
-      </c>
-      <c r="LX6">
-        <v>124</v>
-      </c>
-      <c r="LY6">
-        <v>124</v>
-      </c>
-      <c r="LZ6">
-        <v>123</v>
-      </c>
-      <c r="MA6">
-        <v>123</v>
-      </c>
-      <c r="MB6">
-        <v>122</v>
-      </c>
-      <c r="MC6">
-        <v>121</v>
-      </c>
-      <c r="MD6">
-        <v>121</v>
-      </c>
-      <c r="ME6">
-        <v>119</v>
-      </c>
-      <c r="MF6">
-        <v>118</v>
-      </c>
-      <c r="MG6">
-        <v>118</v>
-      </c>
-      <c r="MH6">
-        <v>117</v>
-      </c>
-      <c r="MI6">
-        <v>117</v>
-      </c>
-      <c r="MJ6">
-        <v>116</v>
-      </c>
-      <c r="MK6">
-        <v>116</v>
-      </c>
-      <c r="ML6">
-        <v>115</v>
-      </c>
-      <c r="MM6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7">
-        <v>129</v>
-      </c>
-      <c r="I7">
-        <v>129</v>
-      </c>
-      <c r="J7">
-        <v>131</v>
-      </c>
-      <c r="K7">
-        <v>132</v>
-      </c>
-      <c r="L7">
-        <v>133</v>
-      </c>
-      <c r="M7">
-        <v>133</v>
-      </c>
-      <c r="N7">
-        <v>134</v>
-      </c>
-      <c r="O7">
-        <v>135</v>
-      </c>
-      <c r="P7">
-        <v>135</v>
-      </c>
-      <c r="Q7">
-        <v>136</v>
-      </c>
-      <c r="R7">
-        <v>136</v>
-      </c>
-      <c r="S7">
-        <v>136</v>
-      </c>
-      <c r="T7">
-        <v>137</v>
-      </c>
-      <c r="U7">
-        <v>137</v>
-      </c>
-      <c r="V7">
-        <v>137</v>
-      </c>
-      <c r="W7">
-        <v>137</v>
-      </c>
-      <c r="X7">
-        <v>137</v>
-      </c>
-      <c r="Y7">
-        <v>137</v>
-      </c>
-      <c r="Z7">
-        <v>137</v>
-      </c>
-      <c r="AA7">
-        <v>137</v>
-      </c>
-      <c r="AB7">
-        <v>137</v>
-      </c>
-      <c r="AC7">
-        <v>137</v>
-      </c>
-      <c r="AD7">
-        <v>136</v>
-      </c>
-      <c r="AE7">
-        <v>135</v>
-      </c>
-      <c r="AF7">
-        <v>133</v>
-      </c>
-      <c r="AG7">
-        <v>133</v>
-      </c>
-      <c r="AH7">
-        <v>131</v>
-      </c>
-      <c r="AI7">
-        <v>130</v>
-      </c>
-      <c r="AJ7">
-        <v>131</v>
-      </c>
-      <c r="AK7">
-        <v>132</v>
-      </c>
-      <c r="AL7">
-        <v>133</v>
-      </c>
-      <c r="AM7">
-        <v>135</v>
-      </c>
-      <c r="AN7">
-        <v>136</v>
-      </c>
-      <c r="AO7">
-        <v>137</v>
-      </c>
-      <c r="AP7">
-        <v>138</v>
-      </c>
-      <c r="AQ7">
-        <v>140</v>
-      </c>
-      <c r="AR7">
-        <v>140</v>
-      </c>
-      <c r="AS7">
-        <v>142</v>
-      </c>
-      <c r="AT7">
-        <v>143</v>
-      </c>
-      <c r="AU7">
-        <v>144</v>
-      </c>
-      <c r="AV7">
-        <v>145</v>
-      </c>
-      <c r="AW7">
-        <v>147</v>
-      </c>
-      <c r="AX7">
-        <v>148</v>
-      </c>
-      <c r="AY7">
-        <v>149</v>
-      </c>
-      <c r="AZ7">
-        <v>150</v>
-      </c>
-      <c r="BA7">
-        <v>151</v>
-      </c>
-      <c r="BB7">
-        <v>152</v>
-      </c>
-      <c r="BC7">
-        <v>150</v>
-      </c>
-      <c r="BD7">
-        <v>148</v>
-      </c>
-      <c r="BE7">
-        <v>146</v>
-      </c>
-      <c r="BF7">
-        <v>144</v>
-      </c>
-      <c r="BG7">
-        <v>142</v>
-      </c>
-      <c r="BH7">
-        <v>140</v>
-      </c>
-      <c r="BI7">
-        <v>138</v>
-      </c>
-      <c r="BJ7">
-        <v>136</v>
-      </c>
-      <c r="BK7">
-        <v>134</v>
-      </c>
-      <c r="BL7">
-        <v>133</v>
-      </c>
-      <c r="BM7">
-        <v>131</v>
-      </c>
-      <c r="BN7">
-        <v>129</v>
-      </c>
-      <c r="BO7">
-        <v>130</v>
-      </c>
-      <c r="BP7">
-        <v>131</v>
-      </c>
-      <c r="BQ7">
-        <v>133</v>
-      </c>
-      <c r="BR7">
-        <v>134</v>
-      </c>
-      <c r="BS7">
-        <v>135</v>
-      </c>
-      <c r="BT7">
-        <v>136</v>
-      </c>
-      <c r="BU7">
-        <v>137</v>
-      </c>
-      <c r="BV7">
-        <v>138</v>
-      </c>
-      <c r="BW7">
-        <v>140</v>
-      </c>
-      <c r="BX7">
-        <v>140</v>
-      </c>
-      <c r="BY7">
-        <v>141</v>
-      </c>
-      <c r="BZ7">
-        <v>143</v>
-      </c>
-      <c r="CA7">
-        <v>144</v>
-      </c>
-      <c r="CB7">
-        <v>145</v>
-      </c>
-      <c r="CC7">
-        <v>145</v>
-      </c>
-      <c r="CD7">
-        <v>147</v>
-      </c>
-      <c r="CE7">
-        <v>148</v>
-      </c>
-      <c r="CF7">
-        <v>146</v>
-      </c>
-      <c r="CG7">
-        <v>144</v>
-      </c>
-      <c r="CH7">
-        <v>142</v>
-      </c>
-      <c r="CI7">
-        <v>140</v>
-      </c>
-      <c r="CJ7">
-        <v>139</v>
-      </c>
-      <c r="CK7">
-        <v>137</v>
-      </c>
-      <c r="CL7">
-        <v>135</v>
-      </c>
-      <c r="CM7">
-        <v>133</v>
-      </c>
-      <c r="CN7">
-        <v>132</v>
-      </c>
-      <c r="CO7">
-        <v>130</v>
-      </c>
-      <c r="CP7">
-        <v>121</v>
-      </c>
-      <c r="CQ7">
-        <v>119</v>
-      </c>
-      <c r="CR7">
-        <v>117</v>
-      </c>
-      <c r="CS7">
-        <v>116</v>
-      </c>
-      <c r="CT7">
-        <v>114</v>
-      </c>
-      <c r="CU7">
-        <v>112</v>
-      </c>
-      <c r="CV7">
-        <v>110</v>
-      </c>
-      <c r="CW7">
-        <v>108</v>
-      </c>
-      <c r="CX7">
-        <v>106</v>
-      </c>
-      <c r="CY7">
-        <v>104</v>
-      </c>
-      <c r="CZ7">
-        <v>104</v>
-      </c>
-      <c r="DA7">
-        <v>102</v>
-      </c>
-      <c r="DB7">
-        <v>101</v>
-      </c>
-      <c r="DC7">
-        <v>100</v>
-      </c>
-      <c r="DD7">
-        <v>99</v>
-      </c>
-      <c r="DE7">
-        <v>99</v>
-      </c>
-      <c r="DF7">
-        <v>98</v>
-      </c>
-      <c r="DG7">
-        <v>97</v>
-      </c>
-      <c r="DH7">
-        <v>96</v>
-      </c>
-      <c r="DI7">
-        <v>95</v>
-      </c>
-      <c r="DJ7">
-        <v>95</v>
-      </c>
-      <c r="DK7">
-        <v>94</v>
-      </c>
-      <c r="DL7">
-        <v>93</v>
-      </c>
-      <c r="DM7">
-        <v>93</v>
-      </c>
-      <c r="DN7">
-        <v>93</v>
-      </c>
-      <c r="DO7">
-        <v>92</v>
-      </c>
-      <c r="DP7">
-        <v>92</v>
-      </c>
-      <c r="DQ7">
-        <v>92</v>
-      </c>
-      <c r="DR7">
-        <v>92</v>
-      </c>
-      <c r="DS7">
-        <v>91</v>
-      </c>
-      <c r="DT7">
-        <v>91</v>
-      </c>
-      <c r="DU7">
-        <v>91</v>
-      </c>
-      <c r="DV7">
-        <v>91</v>
-      </c>
-      <c r="DW7">
-        <v>91</v>
-      </c>
-      <c r="DX7">
-        <v>91</v>
-      </c>
-      <c r="DY7">
-        <v>91</v>
-      </c>
-      <c r="DZ7">
-        <v>91</v>
-      </c>
-      <c r="EA7">
-        <v>91</v>
-      </c>
-      <c r="EB7">
-        <v>91</v>
-      </c>
-      <c r="EC7">
-        <v>91</v>
-      </c>
-      <c r="ED7">
-        <v>91</v>
-      </c>
-      <c r="EE7">
-        <v>91</v>
-      </c>
-      <c r="EF7">
-        <v>91</v>
-      </c>
-      <c r="EG7">
-        <v>92</v>
-      </c>
-      <c r="EH7">
-        <v>92</v>
-      </c>
-      <c r="EI7">
-        <v>93</v>
-      </c>
-      <c r="EJ7">
-        <v>94</v>
-      </c>
-      <c r="EK7">
-        <v>94</v>
-      </c>
-      <c r="EL7">
-        <v>95</v>
-      </c>
-      <c r="EM7">
-        <v>95</v>
-      </c>
-      <c r="EN7">
-        <v>96</v>
-      </c>
-      <c r="EO7">
-        <v>97</v>
-      </c>
-      <c r="EP7">
-        <v>98</v>
-      </c>
-      <c r="EQ7">
-        <v>99</v>
-      </c>
-      <c r="ER7">
-        <v>100</v>
-      </c>
-      <c r="ES7">
-        <v>101</v>
-      </c>
-      <c r="ET7">
-        <v>102</v>
-      </c>
-      <c r="EU7">
-        <v>103</v>
-      </c>
-      <c r="EV7">
-        <v>104</v>
-      </c>
-      <c r="EW7">
-        <v>105</v>
-      </c>
-      <c r="EX7">
-        <v>106</v>
-      </c>
-      <c r="EY7">
-        <v>108</v>
-      </c>
-      <c r="EZ7">
-        <v>110</v>
-      </c>
-      <c r="FA7">
-        <v>111</v>
-      </c>
-      <c r="FB7">
-        <v>112</v>
-      </c>
-      <c r="FC7">
-        <v>114</v>
-      </c>
-      <c r="FD7">
-        <v>116</v>
-      </c>
-      <c r="FE7">
-        <v>117</v>
-      </c>
-      <c r="FF7">
-        <v>119</v>
-      </c>
-      <c r="FG7">
-        <v>121</v>
-      </c>
-      <c r="FH7">
-        <v>122</v>
-      </c>
-      <c r="FI7">
-        <v>110</v>
-      </c>
-      <c r="FJ7">
-        <v>111</v>
-      </c>
-      <c r="FK7">
-        <v>111</v>
-      </c>
-      <c r="FL7">
-        <v>111</v>
-      </c>
-      <c r="FM7">
-        <v>111</v>
-      </c>
-      <c r="FN7">
-        <v>111</v>
-      </c>
-      <c r="FO7">
-        <v>111</v>
-      </c>
-      <c r="FP7">
-        <v>109</v>
-      </c>
-      <c r="FQ7">
-        <v>108</v>
-      </c>
-      <c r="FR7">
-        <v>107</v>
-      </c>
-      <c r="FS7">
-        <v>106</v>
-      </c>
-      <c r="FT7">
-        <v>105</v>
-      </c>
-      <c r="FU7">
-        <v>105</v>
-      </c>
-      <c r="FV7">
-        <v>104</v>
-      </c>
-      <c r="FW7">
-        <v>104</v>
-      </c>
-      <c r="FX7">
-        <v>104</v>
-      </c>
-      <c r="FY7">
-        <v>103</v>
-      </c>
-      <c r="FZ7">
-        <v>103</v>
-      </c>
-      <c r="GA7">
-        <v>105</v>
-      </c>
-      <c r="GB7">
-        <v>106</v>
-      </c>
-      <c r="GC7">
-        <v>108</v>
-      </c>
-      <c r="GD7">
-        <v>110</v>
-      </c>
-      <c r="GE7">
-        <v>110</v>
-      </c>
-      <c r="GF7">
-        <v>110</v>
-      </c>
-      <c r="GG7">
-        <v>111</v>
-      </c>
-      <c r="GH7">
-        <v>111</v>
-      </c>
-      <c r="GI7">
-        <v>112</v>
-      </c>
-      <c r="GJ7">
-        <v>102</v>
-      </c>
-      <c r="GK7">
-        <v>100</v>
-      </c>
-      <c r="GL7">
-        <v>98</v>
-      </c>
-      <c r="GM7">
-        <v>96</v>
-      </c>
-      <c r="GN7">
-        <v>94</v>
-      </c>
-      <c r="GO7">
-        <v>93</v>
-      </c>
-      <c r="GP7">
-        <v>92</v>
-      </c>
-      <c r="GQ7">
-        <v>92</v>
-      </c>
-      <c r="GR7">
-        <v>92</v>
-      </c>
-      <c r="GS7">
-        <v>92</v>
-      </c>
-      <c r="GT7">
-        <v>93</v>
-      </c>
-      <c r="GU7">
-        <v>102</v>
-      </c>
-      <c r="GV7">
-        <v>100</v>
-      </c>
-      <c r="GW7">
-        <v>98</v>
-      </c>
-      <c r="GX7">
-        <v>96</v>
-      </c>
-      <c r="GY7">
-        <v>94</v>
-      </c>
-      <c r="GZ7">
-        <v>93</v>
-      </c>
-      <c r="HA7">
-        <v>92</v>
-      </c>
-      <c r="HB7">
-        <v>92</v>
-      </c>
-      <c r="HC7">
-        <v>92</v>
-      </c>
-      <c r="HD7">
-        <v>92</v>
-      </c>
-      <c r="HE7">
-        <v>110</v>
-      </c>
-      <c r="HF7">
-        <v>110</v>
-      </c>
-      <c r="HG7">
-        <v>109</v>
-      </c>
-      <c r="HH7">
-        <v>109</v>
-      </c>
-      <c r="HI7">
-        <v>108</v>
-      </c>
-      <c r="HJ7">
-        <v>108</v>
-      </c>
-      <c r="HK7">
-        <v>107</v>
-      </c>
-      <c r="HL7">
-        <v>107</v>
-      </c>
-      <c r="HM7">
-        <v>107</v>
-      </c>
-      <c r="HN7">
-        <v>106</v>
-      </c>
-      <c r="HO7">
-        <v>106</v>
-      </c>
-      <c r="HP7">
-        <v>105</v>
-      </c>
-      <c r="HQ7">
-        <v>105</v>
-      </c>
-      <c r="HR7">
-        <v>105</v>
-      </c>
-      <c r="HS7">
-        <v>104</v>
-      </c>
-      <c r="HT7">
-        <v>104</v>
-      </c>
-      <c r="HU7">
-        <v>104</v>
-      </c>
-      <c r="HV7">
-        <v>103</v>
-      </c>
-      <c r="HW7">
-        <v>103</v>
-      </c>
-      <c r="HX7">
-        <v>103</v>
-      </c>
-      <c r="HY7">
-        <v>102</v>
-      </c>
-      <c r="HZ7">
-        <v>101</v>
-      </c>
-      <c r="IA7">
-        <v>101</v>
-      </c>
-      <c r="IB7">
-        <v>101</v>
-      </c>
-      <c r="IC7">
-        <v>100</v>
-      </c>
-      <c r="ID7">
-        <v>100</v>
-      </c>
-      <c r="IE7">
-        <v>100</v>
-      </c>
-      <c r="IF7">
-        <v>100</v>
-      </c>
-      <c r="IG7">
-        <v>104</v>
-      </c>
-      <c r="IH7">
-        <v>103</v>
-      </c>
-      <c r="II7">
-        <v>102</v>
-      </c>
-      <c r="IJ7">
-        <v>102</v>
-      </c>
-      <c r="IK7">
-        <v>101</v>
-      </c>
-      <c r="IL7">
-        <v>100</v>
-      </c>
-      <c r="IM7">
-        <v>100</v>
-      </c>
-      <c r="IN7">
-        <v>99</v>
-      </c>
-      <c r="IO7">
-        <v>99</v>
-      </c>
-      <c r="IP7">
-        <v>98</v>
-      </c>
-      <c r="IQ7">
-        <v>97</v>
-      </c>
-      <c r="IR7">
-        <v>96</v>
-      </c>
-      <c r="IS7">
-        <v>95</v>
-      </c>
-      <c r="IT7">
-        <v>95</v>
-      </c>
-      <c r="IU7">
-        <v>94</v>
-      </c>
-      <c r="IV7">
-        <v>93</v>
-      </c>
-      <c r="IW7">
-        <v>92</v>
-      </c>
-      <c r="IX7">
-        <v>91</v>
-      </c>
-      <c r="IY7">
-        <v>90</v>
-      </c>
-      <c r="IZ7">
-        <v>89</v>
-      </c>
-      <c r="JA7">
-        <v>88</v>
-      </c>
-      <c r="JB7">
-        <v>88</v>
-      </c>
-      <c r="JC7">
-        <v>87</v>
-      </c>
-      <c r="JD7">
-        <v>86</v>
-      </c>
-      <c r="JE7">
-        <v>85</v>
-      </c>
-      <c r="JF7">
-        <v>84</v>
-      </c>
-      <c r="JG7">
-        <v>83</v>
-      </c>
-      <c r="JH7">
-        <v>96</v>
-      </c>
-      <c r="JI7">
-        <v>95</v>
-      </c>
-      <c r="JJ7">
-        <v>94</v>
-      </c>
-      <c r="JK7">
-        <v>93</v>
-      </c>
-      <c r="JL7">
-        <v>92</v>
-      </c>
-      <c r="JM7">
-        <v>91</v>
-      </c>
-      <c r="JN7">
-        <v>90</v>
-      </c>
-      <c r="JO7">
-        <v>89</v>
-      </c>
-      <c r="JP7">
-        <v>88</v>
-      </c>
-      <c r="JQ7">
-        <v>87</v>
-      </c>
-      <c r="JR7">
-        <v>86</v>
-      </c>
-      <c r="JS7">
-        <v>85</v>
-      </c>
-      <c r="JT7">
-        <v>84</v>
-      </c>
-      <c r="JU7">
-        <v>83</v>
-      </c>
-      <c r="JV7">
-        <v>81</v>
-      </c>
-      <c r="JW7">
-        <v>80</v>
-      </c>
-      <c r="JX7">
-        <v>79</v>
-      </c>
-      <c r="JY7">
-        <v>78</v>
-      </c>
-      <c r="JZ7">
-        <v>77</v>
-      </c>
-      <c r="KA7">
-        <v>107</v>
-      </c>
-      <c r="KB7">
-        <v>107</v>
-      </c>
-      <c r="KC7">
-        <v>107</v>
-      </c>
-      <c r="KD7">
-        <v>106</v>
-      </c>
-      <c r="KE7">
-        <v>106</v>
-      </c>
-      <c r="KF7">
-        <v>105</v>
-      </c>
-      <c r="KG7">
-        <v>104</v>
-      </c>
-      <c r="KH7">
-        <v>104</v>
-      </c>
-      <c r="KI7">
-        <v>103</v>
-      </c>
-      <c r="KJ7">
-        <v>103</v>
-      </c>
-      <c r="KK7">
-        <v>103</v>
-      </c>
-      <c r="KL7">
-        <v>102</v>
-      </c>
-      <c r="KM7">
-        <v>102</v>
-      </c>
-      <c r="KN7">
-        <v>101</v>
-      </c>
-      <c r="KO7">
-        <v>101</v>
-      </c>
-      <c r="KP7">
-        <v>100</v>
-      </c>
-      <c r="KQ7">
-        <v>100</v>
-      </c>
-      <c r="KR7">
-        <v>99</v>
-      </c>
-      <c r="KS7">
-        <v>99</v>
-      </c>
-      <c r="KT7">
-        <v>99</v>
-      </c>
-      <c r="KU7">
-        <v>98</v>
-      </c>
-      <c r="KV7">
-        <v>98</v>
-      </c>
-      <c r="KW7">
-        <v>98</v>
-      </c>
-      <c r="KX7">
-        <v>98</v>
-      </c>
-      <c r="KY7">
-        <v>97</v>
-      </c>
-      <c r="KZ7">
-        <v>97</v>
-      </c>
-      <c r="LA7">
-        <v>97</v>
-      </c>
-      <c r="LB7">
-        <v>97</v>
-      </c>
-      <c r="LC7">
-        <v>101</v>
-      </c>
-      <c r="LD7">
-        <v>101</v>
-      </c>
-      <c r="LE7">
-        <v>100</v>
-      </c>
-      <c r="LF7">
-        <v>99</v>
-      </c>
-      <c r="LG7">
-        <v>98</v>
-      </c>
-      <c r="LH7">
-        <v>97</v>
-      </c>
-      <c r="LI7">
-        <v>95</v>
-      </c>
-      <c r="LJ7">
-        <v>94</v>
-      </c>
-      <c r="LK7">
-        <v>93</v>
-      </c>
-      <c r="LL7">
-        <v>92</v>
-      </c>
-      <c r="LM7">
-        <v>91</v>
-      </c>
-      <c r="LN7">
-        <v>90</v>
-      </c>
-      <c r="LO7">
-        <v>89</v>
-      </c>
-      <c r="LP7">
-        <v>88</v>
-      </c>
-      <c r="LQ7">
-        <v>87</v>
-      </c>
-      <c r="LR7">
-        <v>86</v>
-      </c>
-      <c r="LS7">
-        <v>84</v>
-      </c>
-      <c r="LT7">
-        <v>84</v>
-      </c>
-      <c r="LU7">
-        <v>83</v>
-      </c>
-      <c r="LV7">
-        <v>82</v>
-      </c>
-      <c r="LW7">
-        <v>82</v>
-      </c>
-      <c r="LX7">
-        <v>93</v>
-      </c>
-      <c r="LY7">
-        <v>91</v>
-      </c>
-      <c r="LZ7">
-        <v>90</v>
-      </c>
-      <c r="MA7">
-        <v>88</v>
-      </c>
-      <c r="MB7">
-        <v>86</v>
-      </c>
-      <c r="MC7">
-        <v>85</v>
-      </c>
-      <c r="MD7">
-        <v>83</v>
-      </c>
-      <c r="ME7">
-        <v>82</v>
-      </c>
-      <c r="MF7">
-        <v>81</v>
-      </c>
-      <c r="MG7">
-        <v>79</v>
-      </c>
-      <c r="MH7">
-        <v>78</v>
-      </c>
-      <c r="MI7">
-        <v>76</v>
-      </c>
-      <c r="MJ7">
-        <v>75</v>
-      </c>
-      <c r="MK7">
-        <v>73</v>
-      </c>
-      <c r="ML7">
-        <v>72</v>
-      </c>
-      <c r="MM7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="D10">
-        <v>155</v>
-      </c>
-      <c r="E10">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="D11">
-        <v>153</v>
-      </c>
-      <c r="E11">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="D12">
-        <v>153</v>
-      </c>
-      <c r="E12">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="D13">
-        <v>152</v>
-      </c>
-      <c r="E13">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="D14">
-        <v>151</v>
-      </c>
-      <c r="E14">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="D15">
-        <v>149</v>
-      </c>
-      <c r="E15">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="3:351" x14ac:dyDescent="0.3">
-      <c r="D16">
-        <v>148</v>
-      </c>
-      <c r="E16">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17">
-        <v>146</v>
-      </c>
-      <c r="E17">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D18">
-        <v>144</v>
-      </c>
-      <c r="E18">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D19">
-        <v>143</v>
-      </c>
-      <c r="E19">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20">
-        <v>141</v>
-      </c>
-      <c r="E20">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D21">
-        <v>139</v>
-      </c>
-      <c r="E21">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D22">
-        <v>138</v>
-      </c>
-      <c r="E22">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D23">
-        <v>136</v>
-      </c>
-      <c r="E23">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D24">
-        <v>134</v>
-      </c>
-      <c r="E24">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D25">
-        <v>132</v>
-      </c>
-      <c r="E25">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D26">
-        <v>130</v>
-      </c>
-      <c r="E26">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D27">
-        <v>128</v>
-      </c>
-      <c r="E27">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D28">
-        <v>126</v>
-      </c>
-      <c r="E28">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D29">
-        <v>124</v>
-      </c>
-      <c r="E29">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D30">
-        <v>122</v>
-      </c>
-      <c r="E30">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D31">
-        <v>120</v>
-      </c>
-      <c r="E31">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D32">
-        <v>119</v>
-      </c>
-      <c r="E32">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D33">
-        <v>118</v>
-      </c>
-      <c r="E33">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D34">
-        <v>118</v>
-      </c>
-      <c r="E34">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D35">
-        <v>116</v>
-      </c>
-      <c r="E35">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D36">
-        <v>116</v>
-      </c>
-      <c r="E36">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D37">
-        <v>116</v>
-      </c>
-      <c r="E37">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D38">
-        <v>115</v>
-      </c>
-      <c r="E38">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D39">
-        <v>114</v>
-      </c>
-      <c r="E39">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D40">
-        <v>113</v>
-      </c>
-      <c r="E40">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D41">
-        <v>113</v>
-      </c>
-      <c r="E41">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D42">
-        <v>112</v>
-      </c>
-      <c r="E42">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D43">
-        <v>111</v>
-      </c>
-      <c r="E43">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D44">
-        <v>110</v>
-      </c>
-      <c r="E44">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D45">
-        <v>109</v>
-      </c>
-      <c r="E45">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D46">
-        <v>107</v>
-      </c>
-      <c r="E46">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D47">
-        <v>106</v>
-      </c>
-      <c r="E47">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D48">
-        <v>105</v>
-      </c>
-      <c r="E48">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D49">
-        <v>104</v>
-      </c>
-      <c r="E49">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D50">
-        <v>103</v>
-      </c>
-      <c r="E50">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D51">
-        <v>103</v>
-      </c>
-      <c r="E51">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D52">
-        <v>102</v>
-      </c>
-      <c r="E52">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D53">
-        <v>101</v>
-      </c>
-      <c r="E53">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D54">
-        <v>100</v>
-      </c>
-      <c r="E54">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D55">
-        <v>99</v>
-      </c>
-      <c r="E55">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D56">
-        <v>98</v>
-      </c>
-      <c r="E56">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D57">
-        <v>98</v>
-      </c>
-      <c r="E57">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D58">
-        <v>98</v>
-      </c>
-      <c r="E58">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D59">
-        <v>98</v>
-      </c>
-      <c r="E59">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D60">
-        <v>98</v>
-      </c>
-      <c r="E60">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D61">
-        <v>98</v>
-      </c>
-      <c r="E61">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D62">
-        <v>98</v>
-      </c>
-      <c r="E62">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D63">
-        <v>98</v>
-      </c>
-      <c r="E63">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D64">
-        <v>98</v>
-      </c>
-      <c r="E64">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D65">
-        <v>98</v>
-      </c>
-      <c r="E65">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D66">
-        <v>97</v>
-      </c>
-      <c r="E66">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D67">
-        <v>97</v>
-      </c>
-      <c r="E67">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D68">
-        <v>155</v>
-      </c>
-      <c r="E68">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D69">
-        <v>156</v>
-      </c>
-      <c r="E69">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D70">
-        <v>157</v>
-      </c>
-      <c r="E70">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D71">
-        <v>157</v>
-      </c>
-      <c r="E71">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D72">
-        <v>158</v>
-      </c>
-      <c r="E72">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D73">
-        <v>159</v>
-      </c>
-      <c r="E73">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D74">
-        <v>160</v>
-      </c>
-      <c r="E74">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D75">
-        <v>161</v>
-      </c>
-      <c r="E75">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D76">
-        <v>162</v>
-      </c>
-      <c r="E76">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D77">
-        <v>162</v>
-      </c>
-      <c r="E77">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D78">
-        <v>164</v>
-      </c>
-      <c r="E78">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D79">
-        <v>165</v>
-      </c>
-      <c r="E79">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D80">
-        <v>166</v>
-      </c>
-      <c r="E80">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D81">
-        <v>167</v>
-      </c>
-      <c r="E81">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D82">
-        <v>168</v>
-      </c>
-      <c r="E82">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D83">
-        <v>170</v>
-      </c>
-      <c r="E83">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D84">
-        <v>170</v>
-      </c>
-      <c r="E84">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D85">
-        <v>171</v>
-      </c>
-      <c r="E85">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D86">
-        <v>171</v>
-      </c>
-      <c r="E86">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D87">
-        <v>172</v>
-      </c>
-      <c r="E87">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D88">
-        <v>172</v>
-      </c>
-      <c r="E88">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D89">
-        <v>172</v>
-      </c>
-      <c r="E89">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D90">
-        <v>173</v>
-      </c>
-      <c r="E90">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D91">
-        <v>173</v>
-      </c>
-      <c r="E91">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D92">
-        <v>173</v>
-      </c>
-      <c r="E92">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D93">
-        <v>173</v>
-      </c>
-      <c r="E93">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D94">
-        <v>174</v>
-      </c>
-      <c r="E94">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D95">
-        <v>174</v>
-      </c>
-      <c r="E95">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D96">
-        <v>176</v>
-      </c>
-      <c r="E96">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D97">
-        <v>176</v>
-      </c>
-      <c r="E97">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D98">
-        <v>176</v>
-      </c>
-      <c r="E98">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D99">
-        <v>177</v>
-      </c>
-      <c r="E99">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D100">
-        <v>177</v>
-      </c>
-      <c r="E100">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D101">
-        <v>177</v>
-      </c>
-      <c r="E101">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D102">
-        <v>177</v>
-      </c>
-      <c r="E102">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D103">
-        <v>177</v>
-      </c>
-      <c r="E103">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D104">
-        <v>177</v>
-      </c>
-      <c r="E104">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D105">
-        <v>177</v>
-      </c>
-      <c r="E105">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D106">
-        <v>175</v>
-      </c>
-      <c r="E106">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D107">
-        <v>175</v>
-      </c>
-      <c r="E107">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D108">
-        <v>174</v>
-      </c>
-      <c r="E108">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D109">
-        <v>173</v>
-      </c>
-      <c r="E109">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D110">
-        <v>172</v>
-      </c>
-      <c r="E110">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D111">
-        <v>170</v>
-      </c>
-      <c r="E111">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D112">
-        <v>169</v>
-      </c>
-      <c r="E112">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D113">
-        <v>168</v>
-      </c>
-      <c r="E113">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D114">
-        <v>166</v>
-      </c>
-      <c r="E114">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D115">
-        <v>165</v>
-      </c>
-      <c r="E115">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D116">
-        <v>163</v>
-      </c>
-      <c r="E116">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D117">
-        <v>162</v>
-      </c>
-      <c r="E117">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="118" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D118">
-        <v>161</v>
-      </c>
-      <c r="E118">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="119" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D119">
-        <v>159</v>
-      </c>
-      <c r="E119">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="120" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D120">
-        <v>157</v>
-      </c>
-      <c r="E120">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D121">
-        <v>156</v>
-      </c>
-      <c r="E121">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D122">
-        <v>154</v>
-      </c>
-      <c r="E122">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D123">
-        <v>152</v>
-      </c>
-      <c r="E123">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="124" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D124">
-        <v>150</v>
-      </c>
-      <c r="E124">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="125" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D125">
-        <v>149</v>
-      </c>
-      <c r="E125">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="126" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D126">
-        <v>147</v>
-      </c>
-      <c r="E126">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D127">
-        <v>145</v>
-      </c>
-      <c r="E127">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="128" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D128">
-        <v>143</v>
-      </c>
-      <c r="E128">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="129" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D129">
-        <v>141</v>
-      </c>
-      <c r="E129">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="130" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D130">
-        <v>139</v>
-      </c>
-      <c r="E130">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="131" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D131">
-        <v>137</v>
-      </c>
-      <c r="E131">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="132" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D132">
-        <v>135</v>
-      </c>
-      <c r="E132">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="133" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D133">
-        <v>133</v>
-      </c>
-      <c r="E133">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="134" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D134">
-        <v>131</v>
-      </c>
-      <c r="E134">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="135" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D135">
-        <v>129</v>
-      </c>
-      <c r="E135">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="136" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D136">
-        <v>127</v>
-      </c>
-      <c r="E136">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="137" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D137">
-        <v>125</v>
-      </c>
-      <c r="E137">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="138" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D138">
-        <v>123</v>
-      </c>
-      <c r="E138">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="139" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D139">
-        <v>121</v>
-      </c>
-      <c r="E139">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="140" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D140">
-        <v>119</v>
-      </c>
-      <c r="E140">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="141" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D141">
-        <v>117</v>
-      </c>
-      <c r="E141">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="142" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D142">
-        <v>116</v>
-      </c>
-      <c r="E142">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="143" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D143">
-        <v>114</v>
-      </c>
-      <c r="E143">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="144" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D144">
-        <v>113</v>
-      </c>
-      <c r="E144">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D145">
-        <v>111</v>
-      </c>
-      <c r="E145">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D146">
-        <v>110</v>
-      </c>
-      <c r="E146">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D147">
-        <v>108</v>
-      </c>
-      <c r="E147">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="148" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D148">
-        <v>107</v>
-      </c>
-      <c r="E148">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="149" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D149">
-        <v>106</v>
-      </c>
-      <c r="E149">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D150">
-        <v>105</v>
-      </c>
-      <c r="E150">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D151">
-        <v>104</v>
-      </c>
-      <c r="E151">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="152" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D152">
-        <v>103</v>
-      </c>
-      <c r="E152">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="153" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D153">
-        <v>102</v>
-      </c>
-      <c r="E153">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="154" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D154">
-        <v>101</v>
-      </c>
-      <c r="E154">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="155" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D155">
-        <v>100</v>
-      </c>
-      <c r="E155">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="156" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D156">
-        <v>99</v>
-      </c>
-      <c r="E156">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="157" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D157">
-        <v>98</v>
-      </c>
-      <c r="E157">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="158" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D158">
-        <v>98</v>
-      </c>
-      <c r="E158">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="159" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D159">
-        <v>97</v>
-      </c>
-      <c r="E159">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="160" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D160">
-        <v>96</v>
-      </c>
-      <c r="E160">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="161" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D161">
-        <v>96</v>
-      </c>
-      <c r="E161">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="162" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D162">
-        <v>96</v>
-      </c>
-      <c r="E162">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="163" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D163">
-        <v>95</v>
-      </c>
-      <c r="E163">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="164" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D164">
-        <v>95</v>
-      </c>
-      <c r="E164">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="165" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D165">
-        <v>95</v>
-      </c>
-      <c r="E165">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="166" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D166">
-        <v>96</v>
-      </c>
-      <c r="E166">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="167" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D167">
-        <v>139</v>
-      </c>
-      <c r="E167">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="168" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D168">
-        <v>138</v>
-      </c>
-      <c r="E168">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="169" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D169">
-        <v>136</v>
-      </c>
-      <c r="E169">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="170" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D170">
-        <v>134</v>
-      </c>
-      <c r="E170">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="171" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D171">
-        <v>132</v>
-      </c>
-      <c r="E171">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="172" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D172">
-        <v>130</v>
-      </c>
-      <c r="E172">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="173" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D173">
-        <v>128</v>
-      </c>
-      <c r="E173">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="174" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D174">
-        <v>128</v>
-      </c>
-      <c r="E174">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="175" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D175">
-        <v>129</v>
-      </c>
-      <c r="E175">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="176" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D176">
-        <v>130</v>
-      </c>
-      <c r="E176">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D177">
-        <v>131</v>
-      </c>
-      <c r="E177">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D178">
-        <v>132</v>
-      </c>
-      <c r="E178">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D179">
-        <v>134</v>
-      </c>
-      <c r="E179">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="180" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D180">
-        <v>135</v>
-      </c>
-      <c r="E180">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D181">
-        <v>137</v>
-      </c>
-      <c r="E181">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D182">
-        <v>139</v>
-      </c>
-      <c r="E182">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="183" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D183">
-        <v>140</v>
-      </c>
-      <c r="E183">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="184" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D184">
-        <v>142</v>
-      </c>
-      <c r="E184">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="185" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D185">
-        <v>142</v>
-      </c>
-      <c r="E185">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="186" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D186">
-        <v>143</v>
-      </c>
-      <c r="E186">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="187" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D187">
-        <v>143</v>
-      </c>
-      <c r="E187">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="188" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D188">
-        <v>143</v>
-      </c>
-      <c r="E188">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="189" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D189">
-        <v>141</v>
-      </c>
-      <c r="E189">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="190" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D190">
-        <v>139</v>
-      </c>
-      <c r="E190">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="191" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D191">
-        <v>138</v>
-      </c>
-      <c r="E191">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="192" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D192">
-        <v>136</v>
-      </c>
-      <c r="E192">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="193" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D193">
-        <v>135</v>
-      </c>
-      <c r="E193">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="194" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D194">
-        <v>138</v>
-      </c>
-      <c r="E194">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="195" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D195">
-        <v>138</v>
-      </c>
-      <c r="E195">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="196" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D196">
-        <v>138</v>
-      </c>
-      <c r="E196">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="197" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D197">
-        <v>138</v>
-      </c>
-      <c r="E197">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="198" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D198">
-        <v>138</v>
-      </c>
-      <c r="E198">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="199" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D199">
-        <v>137</v>
-      </c>
-      <c r="E199">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="200" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D200">
-        <v>136</v>
-      </c>
-      <c r="E200">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="201" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D201">
-        <v>134</v>
-      </c>
-      <c r="E201">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="202" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D202">
-        <v>132</v>
-      </c>
-      <c r="E202">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="203" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D203">
-        <v>130</v>
-      </c>
-      <c r="E203">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="204" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D204">
-        <v>129</v>
-      </c>
-      <c r="E204">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="205" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D205">
-        <v>139</v>
-      </c>
-      <c r="E205">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="206" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D206">
-        <v>139</v>
-      </c>
-      <c r="E206">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="207" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D207">
-        <v>139</v>
-      </c>
-      <c r="E207">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="208" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D208">
-        <v>139</v>
-      </c>
-      <c r="E208">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="209" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D209">
-        <v>139</v>
-      </c>
-      <c r="E209">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="210" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D210">
-        <v>140</v>
-      </c>
-      <c r="E210">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="211" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D211">
-        <v>141</v>
-      </c>
-      <c r="E211">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="212" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D212">
-        <v>143</v>
-      </c>
-      <c r="E212">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="213" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D213">
-        <v>145</v>
-      </c>
-      <c r="E213">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="214" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D214">
-        <v>147</v>
-      </c>
-      <c r="E214">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="215" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D215">
-        <v>163</v>
-      </c>
-      <c r="E215">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="216" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D216">
-        <v>165</v>
-      </c>
-      <c r="E216">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="217" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D217">
-        <v>166</v>
-      </c>
-      <c r="E217">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="218" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D218">
-        <v>168</v>
-      </c>
-      <c r="E218">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="219" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D219">
-        <v>170</v>
-      </c>
-      <c r="E219">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="220" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D220">
-        <v>172</v>
-      </c>
-      <c r="E220">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="221" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D221">
-        <v>173</v>
-      </c>
-      <c r="E221">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="222" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D222">
-        <v>175</v>
-      </c>
-      <c r="E222">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="223" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D223">
-        <v>177</v>
-      </c>
-      <c r="E223">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="224" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D224">
-        <v>178</v>
-      </c>
-      <c r="E224">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="225" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D225">
-        <v>180</v>
-      </c>
-      <c r="E225">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="226" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D226">
-        <v>181</v>
-      </c>
-      <c r="E226">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="227" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D227">
-        <v>183</v>
-      </c>
-      <c r="E227">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="228" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D228">
-        <v>185</v>
-      </c>
-      <c r="E228">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="229" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D229">
-        <v>186</v>
-      </c>
-      <c r="E229">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="230" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D230">
-        <v>188</v>
-      </c>
-      <c r="E230">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="231" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D231">
-        <v>190</v>
-      </c>
-      <c r="E231">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="232" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D232">
-        <v>191</v>
-      </c>
-      <c r="E232">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="233" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D233">
-        <v>193</v>
-      </c>
-      <c r="E233">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="234" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D234">
-        <v>195</v>
-      </c>
-      <c r="E234">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="235" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D235">
-        <v>197</v>
-      </c>
-      <c r="E235">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="236" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D236">
-        <v>199</v>
-      </c>
-      <c r="E236">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="237" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D237">
-        <v>201</v>
-      </c>
-      <c r="E237">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="238" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D238">
-        <v>203</v>
-      </c>
-      <c r="E238">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="239" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D239">
-        <v>205</v>
-      </c>
-      <c r="E239">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="240" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D240">
-        <v>207</v>
-      </c>
-      <c r="E240">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="241" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D241">
-        <v>209</v>
-      </c>
-      <c r="E241">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="242" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D242">
-        <v>211</v>
-      </c>
-      <c r="E242">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="243" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D243">
-        <v>156</v>
-      </c>
-      <c r="E243">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="244" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D244">
-        <v>157</v>
-      </c>
-      <c r="E244">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="245" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D245">
-        <v>158</v>
-      </c>
-      <c r="E245">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="246" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D246">
-        <v>160</v>
-      </c>
-      <c r="E246">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="247" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D247">
-        <v>161</v>
-      </c>
-      <c r="E247">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="248" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D248">
-        <v>162</v>
-      </c>
-      <c r="E248">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="249" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D249">
-        <v>164</v>
-      </c>
-      <c r="E249">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="250" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D250">
-        <v>165</v>
-      </c>
-      <c r="E250">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="251" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D251">
-        <v>167</v>
-      </c>
-      <c r="E251">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="252" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D252">
-        <v>169</v>
-      </c>
-      <c r="E252">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="253" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D253">
-        <v>170</v>
-      </c>
-      <c r="E253">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="254" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D254">
-        <v>172</v>
-      </c>
-      <c r="E254">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="255" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D255">
-        <v>173</v>
-      </c>
-      <c r="E255">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="256" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D256">
-        <v>175</v>
-      </c>
-      <c r="E256">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="257" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D257">
-        <v>176</v>
-      </c>
-      <c r="E257">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="258" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D258">
-        <v>177</v>
-      </c>
-      <c r="E258">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="259" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D259">
-        <v>179</v>
-      </c>
-      <c r="E259">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="260" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D260">
-        <v>180</v>
-      </c>
-      <c r="E260">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="261" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D261">
-        <v>181</v>
-      </c>
-      <c r="E261">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="262" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D262">
-        <v>183</v>
-      </c>
-      <c r="E262">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="263" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D263">
-        <v>184</v>
-      </c>
-      <c r="E263">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="264" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D264">
-        <v>186</v>
-      </c>
-      <c r="E264">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="265" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D265">
-        <v>187</v>
-      </c>
-      <c r="E265">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="266" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D266">
-        <v>188</v>
-      </c>
-      <c r="E266">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="267" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D267">
-        <v>189</v>
-      </c>
-      <c r="E267">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="268" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D268">
-        <v>190</v>
-      </c>
-      <c r="E268">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="269" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D269">
-        <v>191</v>
-      </c>
-      <c r="E269">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="270" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D270">
-        <v>152</v>
-      </c>
-      <c r="E270">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="271" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D271">
-        <v>153</v>
-      </c>
-      <c r="E271">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="272" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D272">
-        <v>155</v>
-      </c>
-      <c r="E272">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="273" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D273">
-        <v>156</v>
-      </c>
-      <c r="E273">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="274" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D274">
-        <v>157</v>
-      </c>
-      <c r="E274">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="275" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D275">
-        <v>159</v>
-      </c>
-      <c r="E275">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="276" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D276">
-        <v>161</v>
-      </c>
-      <c r="E276">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="277" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D277">
-        <v>162</v>
-      </c>
-      <c r="E277">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="278" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D278">
-        <v>163</v>
-      </c>
-      <c r="E278">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="279" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D279">
-        <v>164</v>
-      </c>
-      <c r="E279">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="280" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D280">
-        <v>165</v>
-      </c>
-      <c r="E280">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="281" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D281">
-        <v>167</v>
-      </c>
-      <c r="E281">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="282" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D282">
-        <v>168</v>
-      </c>
-      <c r="E282">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="283" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D283">
-        <v>169</v>
-      </c>
-      <c r="E283">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="284" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D284">
-        <v>171</v>
-      </c>
-      <c r="E284">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="285" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D285">
-        <v>172</v>
-      </c>
-      <c r="E285">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="286" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D286">
-        <v>173</v>
-      </c>
-      <c r="E286">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="287" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D287">
-        <v>174</v>
-      </c>
-      <c r="E287">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="288" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D288">
-        <v>175</v>
-      </c>
-      <c r="E288">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="289" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D289">
-        <v>114</v>
-      </c>
-      <c r="E289">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="290" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D290">
-        <v>112</v>
-      </c>
-      <c r="E290">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="291" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D291">
-        <v>110</v>
-      </c>
-      <c r="E291">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="292" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D292">
-        <v>109</v>
-      </c>
-      <c r="E292">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="293" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D293">
-        <v>107</v>
-      </c>
-      <c r="E293">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="294" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D294">
-        <v>106</v>
-      </c>
-      <c r="E294">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="295" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D295">
-        <v>105</v>
-      </c>
-      <c r="E295">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="296" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D296">
-        <v>103</v>
-      </c>
-      <c r="E296">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="297" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D297">
-        <v>102</v>
-      </c>
-      <c r="E297">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="298" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D298">
-        <v>100</v>
-      </c>
-      <c r="E298">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="299" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D299">
-        <v>98</v>
-      </c>
-      <c r="E299">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="300" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D300">
-        <v>97</v>
-      </c>
-      <c r="E300">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="301" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D301">
-        <v>95</v>
-      </c>
-      <c r="E301">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="302" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D302">
-        <v>94</v>
-      </c>
-      <c r="E302">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="303" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D303">
-        <v>92</v>
-      </c>
-      <c r="E303">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="304" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D304">
-        <v>91</v>
-      </c>
-      <c r="E304">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="305" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D305">
-        <v>89</v>
-      </c>
-      <c r="E305">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="306" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D306">
-        <v>88</v>
-      </c>
-      <c r="E306">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="307" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D307">
-        <v>86</v>
-      </c>
-      <c r="E307">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="308" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D308">
-        <v>84</v>
-      </c>
-      <c r="E308">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="309" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D309">
-        <v>83</v>
-      </c>
-      <c r="E309">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="310" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D310">
-        <v>81</v>
-      </c>
-      <c r="E310">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="311" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D311">
-        <v>79</v>
-      </c>
-      <c r="E311">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="312" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D312">
-        <v>81</v>
-      </c>
-      <c r="E312">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="313" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D313">
-        <v>82</v>
-      </c>
-      <c r="E313">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="314" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D314">
-        <v>84</v>
-      </c>
-      <c r="E314">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="315" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D315">
-        <v>86</v>
-      </c>
-      <c r="E315">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="316" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D316">
-        <v>88</v>
-      </c>
-      <c r="E316">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="317" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D317">
-        <v>120</v>
-      </c>
-      <c r="E317">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="318" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D318">
-        <v>118</v>
-      </c>
-      <c r="E318">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="319" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D319">
-        <v>117</v>
-      </c>
-      <c r="E319">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="320" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D320">
-        <v>116</v>
-      </c>
-      <c r="E320">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="321" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D321">
-        <v>115</v>
-      </c>
-      <c r="E321">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="322" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D322">
-        <v>114</v>
-      </c>
-      <c r="E322">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="323" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D323">
-        <v>114</v>
-      </c>
-      <c r="E323">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="324" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D324">
-        <v>113</v>
-      </c>
-      <c r="E324">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="325" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D325">
-        <v>112</v>
-      </c>
-      <c r="E325">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="326" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D326">
-        <v>111</v>
-      </c>
-      <c r="E326">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="327" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D327">
-        <v>110</v>
-      </c>
-      <c r="E327">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="328" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D328">
-        <v>109</v>
-      </c>
-      <c r="E328">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="329" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D329">
-        <v>108</v>
-      </c>
-      <c r="E329">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="330" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D330">
-        <v>107</v>
-      </c>
-      <c r="E330">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="331" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D331">
-        <v>106</v>
-      </c>
-      <c r="E331">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="332" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D332">
-        <v>104</v>
-      </c>
-      <c r="E332">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="333" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D333">
-        <v>104</v>
-      </c>
-      <c r="E333">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="334" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D334">
-        <v>102</v>
-      </c>
-      <c r="E334">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="335" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D335">
-        <v>101</v>
-      </c>
-      <c r="E335">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="336" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D336">
-        <v>100</v>
-      </c>
-      <c r="E336">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="337" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D337">
-        <v>98</v>
-      </c>
-      <c r="E337">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="338" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D338">
-        <v>124</v>
-      </c>
-      <c r="E338">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="339" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D339">
-        <v>124</v>
-      </c>
-      <c r="E339">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="340" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D340">
-        <v>123</v>
-      </c>
-      <c r="E340">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="341" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D341">
-        <v>123</v>
-      </c>
-      <c r="E341">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="342" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D342">
-        <v>122</v>
-      </c>
-      <c r="E342">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="343" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D343">
-        <v>121</v>
-      </c>
-      <c r="E343">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="344" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D344">
-        <v>121</v>
-      </c>
-      <c r="E344">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="345" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D345">
-        <v>119</v>
-      </c>
-      <c r="E345">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="346" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D346">
-        <v>118</v>
-      </c>
-      <c r="E346">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="347" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D347">
-        <v>118</v>
-      </c>
-      <c r="E347">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="348" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D348">
-        <v>117</v>
-      </c>
-      <c r="E348">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="349" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D349">
-        <v>117</v>
-      </c>
-      <c r="E349">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="350" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D350">
-        <v>116</v>
-      </c>
-      <c r="E350">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="351" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D351">
-        <v>116</v>
-      </c>
-      <c r="E351">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="352" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D352">
-        <v>115</v>
-      </c>
-      <c r="E352">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="353" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D353">
-        <v>115</v>
-      </c>
-      <c r="E353">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D754114F-8263-40B2-B3C4-9268AA6CC4BD}">
   <dimension ref="B1:H39"/>
   <sheetViews>
@@ -15180,7 +10286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{145B79D5-775D-4E29-9EAD-7B49CEA3F9FE}">
   <dimension ref="A1:T24"/>
   <sheetViews>
@@ -15594,7 +10700,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4196369A-03D1-4C8F-98BD-7201DFB37612}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -15630,7 +10736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEAF763-B173-4EDE-A20E-88549F619A6F}">
   <dimension ref="A1:A5"/>
   <sheetViews>

</xml_diff>

<commit_message>
draw* now draw only, bounce2
New buttons, bounce
draw* now draw only, no timing
</commit_message>
<xml_diff>
--- a/Plots.xlsx
+++ b/Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\O-Scope_XY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20F3CA4-DBC4-47B2-95B3-C8472CCA392E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0C7B51-E4FB-4E11-AABF-826075E30F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3576" yWindow="0" windowWidth="19560" windowHeight="12456" activeTab="1" xr2:uid="{A4021E60-8DFB-4E05-9B04-73E3B9062F1F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>x</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>u</t>
+  </si>
+  <si>
+    <t>Least Comm Denom</t>
+  </si>
+  <si>
+    <t>XY Start</t>
+  </si>
+  <si>
+    <t>XY End</t>
   </si>
 </sst>
 </file>
@@ -6654,8 +6663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E30558C-6DE1-4AFA-9C10-9F4E634DB145}">
   <dimension ref="B1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I49" sqref="G4:I49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6671,6 +6680,25 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>16</v>
@@ -7263,6 +7291,24 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="K35">
+        <f>K31/4</f>
+        <v>6</v>
+      </c>
+      <c r="L35">
+        <f>L31/4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <f t="shared" ref="K36:L36" si="2">K32/4</f>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
@@ -7293,6 +7339,14 @@
       <c r="I37" t="str">
         <f>"// seg "&amp;B37</f>
         <v>// seg p</v>
+      </c>
+      <c r="K37">
+        <f t="shared" ref="K37:L37" si="3">K33/4</f>
+        <v>6</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>